<commit_message>
New datasets & exp. results upd.
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-1.xlsx
+++ b/migforecasting/underground/test-1.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="Тест датасетов" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>train</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>avg</t>
   </si>
@@ -36,16 +30,52 @@
     <t>avg20</t>
   </si>
   <si>
-    <t>Random Forest-100 (citiesdataset-0.xlsx)</t>
-  </si>
-  <si>
     <t>SD20</t>
   </si>
   <si>
-    <t>NN (64,64,64,64,1) (citiesdataset-0.xlsx)</t>
+    <t>train (MAPE)</t>
   </si>
   <si>
-    <t>Критерий MAPE</t>
+    <t>Random Forest-100 (citiesdataset-1.csv)</t>
+  </si>
+  <si>
+    <t>NN (64,64,64,64,1) (citiesdataset-0.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-0.csv)</t>
+  </si>
+  <si>
+    <t>avg50</t>
+  </si>
+  <si>
+    <t>SD50</t>
+  </si>
+  <si>
+    <t>test (MAPE)</t>
+  </si>
+  <si>
+    <t>NN (64,64,64,64,1) (citiesdataset-1.csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-2.csv)</t>
+  </si>
+  <si>
+    <t>NN (64,64,64,64,1) (citiesdataset-2.csv)</t>
+  </si>
+  <si>
+    <t>avgtrain</t>
+  </si>
+  <si>
+    <t>avgtest</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -99,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -110,6 +140,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -125,6 +158,1088 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400"/>
+              <a:t>Тестирование датасетов</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Обучающая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Тест датасетов'!$Q$34:$S$34</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>D0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>D1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>D2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Тест датасетов'!$Q$35:$S$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.19298594523252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375583157465095</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1181073290499999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E6E-469F-8E9E-8E06403940DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Тестовая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Тест датасетов'!$Q$34:$S$34</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>D0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>D1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>D2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Тест датасетов'!$Q$36:$S$36</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.7626578298428059</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1411093366152425</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6907165831152193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8E6E-469F-8E9E-8E06403940DF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="2081397776"/>
+        <c:axId val="2081396112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2081397776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2081396112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2081396112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2081397776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,45 +1505,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:K63"/>
+  <dimension ref="D1:AD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="H25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="10" max="11" width="15" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="19" max="19" width="13.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" customWidth="1"/>
+    <col min="30" max="30" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:30" x14ac:dyDescent="0.25">
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="R2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D4" s="1">
         <v>1</v>
       </c>
@@ -447,8 +1615,36 @@
       <c r="K4" s="3">
         <v>5.0967835174370419</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>2.0166086967244188</v>
+      </c>
+      <c r="O4" s="3">
+        <v>3.3576458004346459</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1.162042413</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>2.1015016463036722</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+    </row>
+    <row r="5" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <f>D4+1</f>
         <v>2</v>
@@ -469,8 +1665,40 @@
       <c r="K5" s="3">
         <v>2.0827175947351448</v>
       </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="1">
+        <f>M4+1</f>
+        <v>2</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1.8048403895128271</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3.232131609009929</v>
+      </c>
+      <c r="R5" s="1">
+        <f>R4+1</f>
+        <v>2</v>
+      </c>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="W5" s="1">
+        <f>W4+1</f>
+        <v>2</v>
+      </c>
+      <c r="X5" s="3">
+        <v>1.045282045</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>3.919665062988869</v>
+      </c>
+      <c r="AB5" s="1">
+        <f>AB4+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+    </row>
+    <row r="6" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <f t="shared" ref="D6:D53" si="0">D5+1</f>
         <v>3</v>
@@ -491,8 +1719,40 @@
       <c r="K6" s="3">
         <v>1.8030520537613419</v>
       </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="1">
+        <f t="shared" ref="M6:M23" si="2">M5+1</f>
+        <v>3</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1.6667150598493199</v>
+      </c>
+      <c r="O6" s="3">
+        <v>1.817072878426959</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" ref="R6:R23" si="3">R5+1</f>
+        <v>3</v>
+      </c>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="W6" s="1">
+        <f t="shared" ref="W6:W23" si="4">W5+1</f>
+        <v>3</v>
+      </c>
+      <c r="X6" s="3">
+        <v>1.100871634</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>1.4531086788752849</v>
+      </c>
+      <c r="AB6" s="1">
+        <f t="shared" ref="AB6:AB23" si="5">AB5+1</f>
+        <v>3</v>
+      </c>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+    </row>
+    <row r="7" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -513,8 +1773,40 @@
       <c r="K7" s="3">
         <v>3.005330368905081</v>
       </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="1">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N7" s="3">
+        <v>2.098681335140641</v>
+      </c>
+      <c r="O7" s="3">
+        <v>2.4309099072945122</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="W7" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="X7" s="3">
+        <v>1.0995125530000001</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>1.8600276753537699</v>
+      </c>
+      <c r="AB7" s="1">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+    </row>
+    <row r="8" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -535,8 +1827,40 @@
       <c r="K8" s="3">
         <v>2.0966012558065419</v>
       </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="1">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="N8" s="3">
+        <v>2.0928360757667752</v>
+      </c>
+      <c r="O8" s="3">
+        <v>4.3618126058758202</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="W8" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="X8" s="3">
+        <v>1.154169325</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>1.452689465878616</v>
+      </c>
+      <c r="AB8" s="1">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+    </row>
+    <row r="9" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -557,8 +1881,40 @@
       <c r="K9" s="3">
         <v>9.4111431585753618</v>
       </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="1">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1.94488781146292</v>
+      </c>
+      <c r="O9" s="3">
+        <v>2.911553580846463</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="W9" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="X9" s="3">
+        <v>1.1805436540000001</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>1.6683692397657079</v>
+      </c>
+      <c r="AB9" s="1">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+    </row>
+    <row r="10" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -579,8 +1935,40 @@
       <c r="K10" s="3">
         <v>4.1744304858058978</v>
       </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="1">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1.9459959635721209</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1.7432350290119589</v>
+      </c>
+      <c r="R10" s="1">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="W10" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="X10" s="3">
+        <v>1.09383499</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>2.0737955956040199</v>
+      </c>
+      <c r="AB10" s="1">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+    </row>
+    <row r="11" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -601,8 +1989,40 @@
       <c r="K11" s="3">
         <v>3.5036446267811119</v>
       </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M11" s="1">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N11" s="3">
+        <v>2.017251485373468</v>
+      </c>
+      <c r="O11" s="3">
+        <v>3.4831126696534001</v>
+      </c>
+      <c r="R11" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="W11" s="1">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="X11" s="3">
+        <v>1.1649971219999999</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>3.6721057154438341</v>
+      </c>
+      <c r="AB11" s="1">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+    </row>
+    <row r="12" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -623,8 +2043,40 @@
       <c r="K12" s="3">
         <v>7.8723253126132926</v>
       </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M12" s="1">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2.0763408587895609</v>
+      </c>
+      <c r="O12" s="3">
+        <v>5.9774142004261668</v>
+      </c>
+      <c r="R12" s="1">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="W12" s="1">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="X12" s="3">
+        <v>1.1801815840000001</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>1.2760919746087329</v>
+      </c>
+      <c r="AB12" s="1">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+    </row>
+    <row r="13" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -645,8 +2097,40 @@
       <c r="K13" s="3">
         <v>2.733601292749483</v>
       </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M13" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1.815059848201217</v>
+      </c>
+      <c r="O13" s="3">
+        <v>2.2577485513990752</v>
+      </c>
+      <c r="R13" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="W13" s="1">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0.93446213600000005</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>8.9051512022220756</v>
+      </c>
+      <c r="AB13" s="1">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+    </row>
+    <row r="14" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -667,8 +2151,40 @@
       <c r="K14" s="3">
         <v>3.4902613807534828</v>
       </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M14" s="1">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1.6920230511004559</v>
+      </c>
+      <c r="O14" s="3">
+        <v>7.339829308029076</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="W14" s="1">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="X14" s="3">
+        <v>1.1575765499999999</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>1.7739776325922041</v>
+      </c>
+      <c r="AB14" s="1">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+    </row>
+    <row r="15" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -689,8 +2205,40 @@
       <c r="K15" s="3">
         <v>5.5262351805627379</v>
       </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M15" s="1">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1.863260732421234</v>
+      </c>
+      <c r="O15" s="3">
+        <v>1.565113708581229</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="W15" s="1">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="X15" s="3">
+        <v>1.214320029</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>1.987626116081725</v>
+      </c>
+      <c r="AB15" s="1">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+    </row>
+    <row r="16" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -711,8 +2259,40 @@
       <c r="K16" s="3">
         <v>3.0299325566033928</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M16" s="1">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="N16" s="3">
+        <v>2.0837153141583791</v>
+      </c>
+      <c r="O16" s="3">
+        <v>1.6385969337937749</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="W16" s="1">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="X16" s="3">
+        <v>1.0562403739999999</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>1.8660867448759619</v>
+      </c>
+      <c r="AB16" s="1">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+    </row>
+    <row r="17" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -733,8 +2313,40 @@
       <c r="K17" s="3">
         <v>2.3550797926548381</v>
       </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M17" s="1">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="N17" s="3">
+        <v>2.0758520312485702</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1.9960964146064171</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="W17" s="1">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="X17" s="3">
+        <v>1.144334287</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>1.5698264895467831</v>
+      </c>
+      <c r="AB17" s="1">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+    </row>
+    <row r="18" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -755,8 +2367,40 @@
       <c r="K18" s="3">
         <v>2.1095447695979859</v>
       </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M18" s="1">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="N18" s="3">
+        <v>1.8998516900227771</v>
+      </c>
+      <c r="O18" s="3">
+        <v>8.5762432534899382</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="W18" s="1">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0.87991298600000001</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>6.7453926000913782</v>
+      </c>
+      <c r="AB18" s="1">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+    </row>
+    <row r="19" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -777,8 +2421,40 @@
       <c r="K19" s="3">
         <v>2.1765104061379201</v>
       </c>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M19" s="1">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="N19" s="3">
+        <v>1.7955421000626841</v>
+      </c>
+      <c r="O19" s="3">
+        <v>5.7590970765334131</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="W19" s="1">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="X19" s="3">
+        <v>1.2078220319999999</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>2.6221510831318509</v>
+      </c>
+      <c r="AB19" s="1">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+    </row>
+    <row r="20" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -799,8 +2475,40 @@
       <c r="K20" s="3">
         <v>1.8722691315333271</v>
       </c>
-    </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M20" s="1">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="N20" s="3">
+        <v>1.9237063054879171</v>
+      </c>
+      <c r="O20" s="3">
+        <v>2.571117403937643</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="W20" s="1">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="X20" s="3">
+        <v>1.1861801219999999</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>2.252190023459971</v>
+      </c>
+      <c r="AB20" s="1">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+    </row>
+    <row r="21" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -821,8 +2529,40 @@
       <c r="K21" s="3">
         <v>3.9979345805716582</v>
       </c>
-    </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M21" s="1">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1.9034772091336269</v>
+      </c>
+      <c r="O21" s="3">
+        <v>11.227159925611691</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="W21" s="1">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="X21" s="3">
+        <v>1.1364969009999999</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>2.8395707412786728</v>
+      </c>
+      <c r="AB21" s="1">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D22" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -843,8 +2583,40 @@
       <c r="K22" s="3">
         <v>2.942497848777017</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M22" s="1">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="N22" s="3">
+        <v>1.8319808475653141</v>
+      </c>
+      <c r="O22" s="3">
+        <v>7.5962356821654646</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="W22" s="1">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="X22" s="3">
+        <v>1.1900894129999999</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>2.1352673383788572</v>
+      </c>
+      <c r="AB22" s="1">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+    </row>
+    <row r="23" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D23" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -865,8 +2637,40 @@
       <c r="K23" s="3">
         <v>4.4715271372758814</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M23" s="1">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="N23" s="3">
+        <v>2.2025395093359639</v>
+      </c>
+      <c r="O23" s="3">
+        <v>2.9800601931772719</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="W23" s="1">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="X23" s="3">
+        <v>1.073276431</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>1.639736635822387</v>
+      </c>
+      <c r="AB23" s="1">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+    </row>
+    <row r="24" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D24" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -888,7 +2692,7 @@
         <v>11.471393603647069</v>
       </c>
     </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D25" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -909,8 +2713,40 @@
       <c r="K25" s="3">
         <v>1.6879520281866529</v>
       </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="3">
+        <f>AVERAGE(N4:N23)</f>
+        <v>1.9375583157465095</v>
+      </c>
+      <c r="O25" s="3">
+        <f>AVERAGE(O4:O23)</f>
+        <v>4.1411093366152425</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="W25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X25" s="3">
+        <f>AVERAGE(X4:X23)</f>
+        <v>1.1181073290499999</v>
+      </c>
+      <c r="Y25" s="3">
+        <f>AVERAGE(Y4:Y23)</f>
+        <v>2.6907165831152193</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+    </row>
+    <row r="26" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D26" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -931,8 +2767,40 @@
       <c r="K26" s="3">
         <v>2.8982134159016111</v>
       </c>
-    </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="M26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3">
+        <f>_xlfn.STDEV.S(N4:N23)</f>
+        <v>0.14484718308042885</v>
+      </c>
+      <c r="O26" s="3">
+        <f>_xlfn.STDEV.S(O4:O23)</f>
+        <v>2.7184627461630066</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="W26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X26" s="3">
+        <f>_xlfn.STDEV.S(X4:X23)</f>
+        <v>8.7575723830739929E-2</v>
+      </c>
+      <c r="Y26" s="3">
+        <f>_xlfn.STDEV.S(Y4:Y23)</f>
+        <v>1.9189496566065407</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+    </row>
+    <row r="27" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D27" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -954,7 +2822,7 @@
         <v>6.3956052066152944</v>
       </c>
     </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D28" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -976,7 +2844,7 @@
         <v>7.9492698680917302</v>
       </c>
     </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D29" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -998,7 +2866,7 @@
         <v>10.657572144694941</v>
       </c>
     </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D30" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1020,7 +2888,7 @@
         <v>1.739650677783058</v>
       </c>
     </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D31" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1042,7 +2910,7 @@
         <v>5.6688597232590476</v>
       </c>
     </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D32" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1064,7 +2932,7 @@
         <v>2.3210446319047011</v>
       </c>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D33" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1086,7 +2954,7 @@
         <v>2.804279288403654</v>
       </c>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D34" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1107,8 +2975,18 @@
       <c r="K34" s="3">
         <v>2.759626922645845</v>
       </c>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D35" s="1">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1129,8 +3007,20 @@
       <c r="K35" s="3">
         <v>1.8563843382143099</v>
       </c>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="P35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q35" s="6">
+        <v>2.19298594523252</v>
+      </c>
+      <c r="R35" s="6">
+        <v>1.9375583157465095</v>
+      </c>
+      <c r="S35" s="6">
+        <v>1.1181073290499999</v>
+      </c>
+    </row>
+    <row r="36" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D36" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1151,8 +3041,20 @@
       <c r="K36" s="3">
         <v>1.545905783972747</v>
       </c>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="P36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q36" s="6">
+        <v>4.7626578298428059</v>
+      </c>
+      <c r="R36" s="6">
+        <v>4.1411093366152425</v>
+      </c>
+      <c r="S36" s="6">
+        <v>2.6907165831152193</v>
+      </c>
+    </row>
+    <row r="37" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D37" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1174,7 +3076,7 @@
         <v>9.1006326308409182</v>
       </c>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D38" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1196,7 +3098,7 @@
         <v>2.8146111149340061</v>
       </c>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D39" s="1">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1218,7 +3120,7 @@
         <v>6.7935904086275194</v>
       </c>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D40" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1240,7 +3142,7 @@
         <v>3.0454186897591322</v>
       </c>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D41" s="1">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1262,7 +3164,7 @@
         <v>2.0836804357714942</v>
       </c>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D42" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1284,7 +3186,7 @@
         <v>3.391447795174571</v>
       </c>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D43" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1306,7 +3208,7 @@
         <v>4.8857494288124776</v>
       </c>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D44" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1328,7 +3230,7 @@
         <v>2.054671002452741</v>
       </c>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D45" s="1">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1350,7 +3252,7 @@
         <v>2.9436119516446269</v>
       </c>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D46" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1372,7 +3274,7 @@
         <v>2.2483340993940168</v>
       </c>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D47" s="1">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1394,7 +3296,7 @@
         <v>7.3121925986078713</v>
       </c>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D48" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1528,7 +3430,7 @@
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D55" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E55" s="3">
         <f>AVERAGE(E4:E53)</f>
@@ -1539,7 +3441,7 @@
         <v>4.7808843010861146</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J55" s="3">
         <f>AVERAGE(J4:J53)</f>
@@ -1552,7 +3454,7 @@
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E56" s="3">
         <f>_xlfn.STDEV.S(E4:E55)</f>
@@ -1563,7 +3465,7 @@
         <v>3.7215122258269755</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J56" s="3">
         <f>_xlfn.STDEV.S(J4:J55)</f>
@@ -1584,7 +3486,7 @@
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D58" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E58" s="3">
         <f>AVERAGE(E4:E23)</f>
@@ -1595,7 +3497,7 @@
         <v>4.7626578298428059</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J58" s="3">
         <f>AVERAGE(J4:J23)</f>
@@ -1608,7 +3510,7 @@
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D59" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E59" s="3">
         <f>_xlfn.STDEV.S(E4:E23)</f>
@@ -1619,7 +3521,7 @@
         <v>4.3633644798805014</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J59" s="3">
         <f>_xlfn.STDEV.S(J4:J23)</f>
@@ -1645,5 +3547,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NN test on dataset-1
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-1.xlsx
+++ b/migforecasting/underground/test-1.xlsx
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:AD63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF26" sqref="AF26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,8 +1627,12 @@
       <c r="R4" s="1">
         <v>1</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
+      <c r="S4" s="3">
+        <v>2.3338817159762728</v>
+      </c>
+      <c r="T4" s="3">
+        <v>1.844426143127708</v>
+      </c>
       <c r="W4" s="1">
         <v>1</v>
       </c>
@@ -1679,8 +1683,12 @@
         <f>R4+1</f>
         <v>2</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="S5" s="3">
+        <v>1.8396662312479291</v>
+      </c>
+      <c r="T5" s="3">
+        <v>2.898220183133986</v>
+      </c>
       <c r="W5" s="1">
         <f>W4+1</f>
         <v>2</v>
@@ -1733,8 +1741,12 @@
         <f t="shared" ref="R6:R23" si="3">R5+1</f>
         <v>3</v>
       </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
+      <c r="S6" s="3">
+        <v>2.6832698447032728</v>
+      </c>
+      <c r="T6" s="3">
+        <v>2.5747925879576421</v>
+      </c>
       <c r="W6" s="1">
         <f t="shared" ref="W6:W23" si="4">W5+1</f>
         <v>3</v>
@@ -1787,8 +1799,12 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
+      <c r="S7" s="3">
+        <v>2.5560328331158351</v>
+      </c>
+      <c r="T7" s="3">
+        <v>4.1262811741880876</v>
+      </c>
       <c r="W7" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
@@ -1841,8 +1857,12 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="S8" s="3">
+        <v>2.130629583818636</v>
+      </c>
+      <c r="T8" s="3">
+        <v>2.174855434444773</v>
+      </c>
       <c r="W8" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -1895,8 +1915,12 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
+      <c r="S9" s="3">
+        <v>2.1367701992429531</v>
+      </c>
+      <c r="T9" s="3">
+        <v>2.8717321863135301</v>
+      </c>
       <c r="W9" s="1">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -1949,8 +1973,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
+      <c r="S10" s="3">
+        <v>1.92050790082374</v>
+      </c>
+      <c r="T10" s="3">
+        <v>6.3663036506270876</v>
+      </c>
       <c r="W10" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
@@ -2003,8 +2031,12 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
+      <c r="S11" s="3">
+        <v>2.0474093052567781</v>
+      </c>
+      <c r="T11" s="3">
+        <v>2.0402131088053679</v>
+      </c>
       <c r="W11" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
@@ -2057,8 +2089,12 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="S12" s="3">
+        <v>1.9040628265116191</v>
+      </c>
+      <c r="T12" s="3">
+        <v>2.1729117188903819</v>
+      </c>
       <c r="W12" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
@@ -2111,8 +2147,12 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
+      <c r="S13" s="3">
+        <v>2.158731334582503</v>
+      </c>
+      <c r="T13" s="3">
+        <v>3.0445896917428339</v>
+      </c>
       <c r="W13" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
@@ -2165,8 +2205,12 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
+      <c r="S14" s="3">
+        <v>2.1653477504282299</v>
+      </c>
+      <c r="T14" s="3">
+        <v>2.8508723057229748</v>
+      </c>
       <c r="W14" s="1">
         <f t="shared" si="4"/>
         <v>11</v>
@@ -2219,8 +2263,12 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
+      <c r="S15" s="3">
+        <v>1.815639288814815</v>
+      </c>
+      <c r="T15" s="3">
+        <v>2.6667692290704879</v>
+      </c>
       <c r="W15" s="1">
         <f t="shared" si="4"/>
         <v>12</v>
@@ -2273,8 +2321,12 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
+      <c r="S16" s="3">
+        <v>2.13641541998236</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1.7513266206440681</v>
+      </c>
       <c r="W16" s="1">
         <f t="shared" si="4"/>
         <v>13</v>
@@ -2327,8 +2379,12 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="S17" s="3"/>
-      <c r="T17" s="3"/>
+      <c r="S17" s="3">
+        <v>2.0677706749864031</v>
+      </c>
+      <c r="T17" s="3">
+        <v>3.8699078755347069</v>
+      </c>
       <c r="W17" s="1">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -2381,8 +2437,12 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
+      <c r="S18" s="3">
+        <v>1.6608359499970731</v>
+      </c>
+      <c r="T18" s="3">
+        <v>8.2983822503209286</v>
+      </c>
       <c r="W18" s="1">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -2435,8 +2495,12 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
+      <c r="S19" s="3">
+        <v>1.423836789774076</v>
+      </c>
+      <c r="T19" s="3">
+        <v>7.3366965566606037</v>
+      </c>
       <c r="W19" s="1">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -2489,8 +2553,12 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
+      <c r="S20" s="3">
+        <v>2.388303879367482</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1.774771100212797</v>
+      </c>
       <c r="W20" s="1">
         <f t="shared" si="4"/>
         <v>17</v>
@@ -2543,8 +2611,12 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="S21" s="3">
+        <v>2.1199140455566901</v>
+      </c>
+      <c r="T21" s="3">
+        <v>2.2196718036937231</v>
+      </c>
       <c r="W21" s="1">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -2597,8 +2669,12 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="S22" s="3"/>
-      <c r="T22" s="3"/>
+      <c r="S22" s="3">
+        <v>2.5710529058009661</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1.639812421188751</v>
+      </c>
       <c r="W22" s="1">
         <f t="shared" si="4"/>
         <v>19</v>
@@ -2651,8 +2727,12 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
+      <c r="S23" s="3">
+        <v>2.1234460015807608</v>
+      </c>
+      <c r="T23" s="3">
+        <v>1.4706705227527821</v>
+      </c>
       <c r="W23" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
@@ -2727,8 +2807,14 @@
       <c r="R25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3"/>
+      <c r="S25" s="3">
+        <f>AVERAGE(S4:S23)</f>
+        <v>2.10917622407842</v>
+      </c>
+      <c r="T25" s="3">
+        <f>AVERAGE(T4:T23)</f>
+        <v>3.1996603282516611</v>
+      </c>
       <c r="W25" s="1" t="s">
         <v>0</v>
       </c>
@@ -2781,8 +2867,14 @@
       <c r="R26" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
+      <c r="S26" s="3">
+        <f>_xlfn.STDEV.S(S4:S23)</f>
+        <v>0.3070734729535422</v>
+      </c>
+      <c r="T26" s="3">
+        <f>_xlfn.STDEV.S(T4:T23)</f>
+        <v>1.9366596505673197</v>
+      </c>
       <c r="W26" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>